<commit_message>
kayıt data hatası giderildi
</commit_message>
<xml_diff>
--- a/insta.xlsx
+++ b/insta.xlsx
@@ -1,36 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="585" windowWidth="23340" windowHeight="11955"/>
+    <workbookView activeTab="0" windowHeight="11955" windowWidth="23340" xWindow="630" yWindow="585"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">
+____________&lt;TK&gt;____________ (@tlgkyck) • Instagram photos and videos
+</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,21 +53,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -348,15 +349,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hata döndürme düzenlemesi yapıldı
</commit_message>
<xml_diff>
--- a/insta.xlsx
+++ b/insta.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" windowHeight="11955" windowWidth="23340" xWindow="630" yWindow="585"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -59,7 +60,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -356,8 +357,8 @@
   </sheetPr>
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Date time paragraf atlama sorunu düzeltildi
</commit_message>
<xml_diff>
--- a/insta.xlsx
+++ b/insta.xlsx
@@ -26,7 +26,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -56,8 +58,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -355,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -363,11 +366,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="K1" s="1" t="n">
+        <v>43147.51219534304</v>
+      </c>
       <c r="P1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Değişikliklerin koda yazdırılması eklendi
</commit_message>
<xml_diff>
--- a/insta.xlsx
+++ b/insta.xlsx
@@ -2,23 +2,27 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" windowHeight="12210" windowWidth="27660" xWindow="630" yWindow="555"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t xml:space="preserve">
 ____________&lt;TK&gt;____________ (@tlgkyck) • Instagram photos and videos
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+okul (@tlgkyck) • Instagram photos and videos
 </t>
   </si>
 </sst>
@@ -26,8 +30,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+  <numFmts count="2">
+    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="165"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -58,12 +63,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -358,26 +364,42 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="11" min="11" width="18.28515625"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="1" t="n">
-        <v>43147.51219534304</v>
-      </c>
-      <c r="P1" t="s">
-        <v>0</v>
+        <v>43147.51219907407</v>
       </c>
       <c r="Z1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>43147.56716963602</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>43147.56776974755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>